<commit_message>
Added Code in Interview Questions page
</commit_message>
<xml_diff>
--- a/data/matching_profiles.xlsx
+++ b/data/matching_profiles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:H1"/>
+  <dimension ref="B1:AF1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,35 +436,155 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.24</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.23</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.22</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.21</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.20</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.19</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.18</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.17</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.16</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.15</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.14</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.13</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.12</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.11</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.10</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.9</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.8</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.7</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.6</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.5</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.4</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.3</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.2</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Applicant_Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>years_of_exp</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Key_Skills</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Linkedin_Profile</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>GitHub_Profile</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Mail_Id</t>
         </is>

</xml_diff>